<commit_message>
Format the output XLSX files' column sizes
</commit_message>
<xml_diff>
--- a/Reports/administrative_business_development.xlsx
+++ b/Reports/administrative_business_development.xlsx
@@ -1,20 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vchov\workspace\lansweeper\Reports\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView activeTab="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
   </bookViews>
   <sheets>
-    <sheet name="Tablib Dataset" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Tablib Dataset" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>TicketID</t>
   </si>
@@ -43,23 +48,24 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -75,16 +81,25 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -372,21 +387,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane activePane="bottomLeft" state="frozen" topLeftCell="A2" ySplit="1"/>
-      <selection activeCell="A1" pane="bottomLeft" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="43.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.42578125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -400,7 +417,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -415,6 +432,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>